<commit_message>
show details and save to excel
</commit_message>
<xml_diff>
--- a/קבצי אקסל/לקוחות ביתיים.xlsx
+++ b/קבצי אקסל/לקוחות ביתיים.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -399,7 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -510,7 +510,7 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>חסר</v>
+        <v>רות קורן</v>
       </c>
       <c r="B3" t="str">
         <v>חסר</v>

</xml_diff>

<commit_message>
complete beiti and iski before add fix to iski
</commit_message>
<xml_diff>
--- a/קבצי אקסל/לקוחות ביתיים.xlsx
+++ b/קבצי אקסל/לקוחות ביתיים.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -443,27 +443,39 @@
         <v>קומה</v>
       </c>
       <c r="N1" t="str">
+        <v>שם בעל הכרטיס</v>
+      </c>
+      <c r="O1" t="str">
+        <v>מספר זהות/דרכון</v>
+      </c>
+      <c r="P1" t="str">
+        <v>מספר כרטיס</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>תוקף</v>
+      </c>
+      <c r="R1" t="str">
         <v>מספר חוזה</v>
       </c>
-      <c r="O1" t="str">
+      <c r="S1" t="str">
         <v>מספר מונה</v>
       </c>
-      <c r="P1" t="str">
+      <c r="T1" t="str">
         <v>סוג התעריף</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="U1" t="str">
         <v>שם בן הזוג</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>רות קורן</v>
+        <v>חני</v>
       </c>
       <c r="B2" t="str">
         <v>רות</v>
       </c>
       <c r="C2" t="str">
-        <v>קורן</v>
+        <v/>
       </c>
       <c r="D2" t="str">
         <v/>
@@ -502,21 +514,33 @@
         <v/>
       </c>
       <c r="P2" t="str">
+        <v/>
+      </c>
+      <c r="Q2" t="str">
+        <v/>
+      </c>
+      <c r="R2" t="str">
+        <v/>
+      </c>
+      <c r="S2" t="str">
+        <v/>
+      </c>
+      <c r="T2" t="str">
         <v>ג</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="U2" t="str">
         <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>רות קורן</v>
+        <v>מאיר</v>
       </c>
       <c r="B3" t="str">
-        <v>רות</v>
+        <v>חנה</v>
       </c>
       <c r="C3" t="str">
-        <v>קלויורן</v>
+        <v>כהן</v>
       </c>
       <c r="D3" t="str">
         <v/>
@@ -555,174 +579,27 @@
         <v/>
       </c>
       <c r="P3" t="str">
+        <v/>
+      </c>
+      <c r="Q3" t="str">
+        <v/>
+      </c>
+      <c r="R3" t="str">
+        <v/>
+      </c>
+      <c r="S3" t="str">
+        <v/>
+      </c>
+      <c r="T3" t="str">
         <v>ג</v>
       </c>
-      <c r="Q3" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>רות קורן</v>
-      </c>
-      <c r="B4" t="str">
-        <v>רות</v>
-      </c>
-      <c r="C4" t="str">
-        <v>קלויורן</v>
-      </c>
-      <c r="D4" t="str">
-        <v/>
-      </c>
-      <c r="E4" t="str">
-        <v/>
-      </c>
-      <c r="F4" t="str">
-        <v/>
-      </c>
-      <c r="G4" t="str">
-        <v>לא</v>
-      </c>
-      <c r="H4" t="str">
-        <v/>
-      </c>
-      <c r="I4" t="str">
-        <v/>
-      </c>
-      <c r="J4" t="str">
-        <v/>
-      </c>
-      <c r="K4" t="str">
-        <v/>
-      </c>
-      <c r="L4" t="str">
-        <v/>
-      </c>
-      <c r="M4" t="str">
-        <v/>
-      </c>
-      <c r="N4" t="str">
-        <v/>
-      </c>
-      <c r="O4" t="str">
-        <v/>
-      </c>
-      <c r="P4" t="str">
-        <v>ג</v>
-      </c>
-      <c r="Q4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>רות קורן</v>
-      </c>
-      <c r="B5" t="str">
-        <v>רות</v>
-      </c>
-      <c r="C5" t="str">
-        <v>קלויורן</v>
-      </c>
-      <c r="D5" t="str">
-        <v/>
-      </c>
-      <c r="E5" t="str">
-        <v/>
-      </c>
-      <c r="F5" t="str">
-        <v/>
-      </c>
-      <c r="G5" t="str">
-        <v>לא</v>
-      </c>
-      <c r="H5" t="str">
-        <v/>
-      </c>
-      <c r="I5" t="str">
-        <v/>
-      </c>
-      <c r="J5" t="str">
-        <v/>
-      </c>
-      <c r="K5" t="str">
-        <v/>
-      </c>
-      <c r="L5" t="str">
-        <v/>
-      </c>
-      <c r="M5" t="str">
-        <v/>
-      </c>
-      <c r="N5" t="str">
-        <v/>
-      </c>
-      <c r="O5" t="str">
-        <v/>
-      </c>
-      <c r="P5" t="str">
-        <v>ג</v>
-      </c>
-      <c r="Q5" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>רות קורן</v>
-      </c>
-      <c r="B6" t="str">
-        <v>רות</v>
-      </c>
-      <c r="C6" t="str">
-        <v>קלויורן</v>
-      </c>
-      <c r="D6" t="str">
-        <v/>
-      </c>
-      <c r="E6" t="str">
-        <v/>
-      </c>
-      <c r="F6" t="str">
-        <v/>
-      </c>
-      <c r="G6" t="str">
-        <v>לא</v>
-      </c>
-      <c r="H6" t="str">
-        <v/>
-      </c>
-      <c r="I6" t="str">
-        <v/>
-      </c>
-      <c r="J6" t="str">
-        <v/>
-      </c>
-      <c r="K6" t="str">
-        <v/>
-      </c>
-      <c r="L6" t="str">
-        <v/>
-      </c>
-      <c r="M6" t="str">
-        <v/>
-      </c>
-      <c r="N6" t="str">
-        <v/>
-      </c>
-      <c r="O6" t="str">
-        <v>123456789</v>
-      </c>
-      <c r="P6" t="str">
-        <v>ג</v>
-      </c>
-      <c r="Q6" t="str">
+      <c r="U3" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:U3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
function works for both fix
</commit_message>
<xml_diff>
--- a/קבצי אקסל/לקוחות ביתיים.xlsx
+++ b/קבצי אקסל/לקוחות ביתיים.xlsx
@@ -399,7 +399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -475,7 +475,7 @@
         <v>רות</v>
       </c>
       <c r="C2" t="str">
-        <v/>
+        <v>kuhi</v>
       </c>
       <c r="D2" t="str">
         <v/>

</xml_diff>